<commit_message>
Plan de auditoria corregido
</commit_message>
<xml_diff>
--- a/06 Plan de Auditoria/PROGRAMA_AUDIT_INTERNA.xlsx
+++ b/06 Plan de Auditoria/PROGRAMA_AUDIT_INTERNA.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dylan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANDRES\OneDrive\Documents\14937_G2_ACS\06 Plan de Auditoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DBD4B5E1-18DA-427B-8341-3F15E79B8FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{AA0757F3-7C9A-43E8-AE92-280E31840668}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1, PROGRAMA" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'2. PLAN DE AUDITORIA'!$2:$14</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'3.CHECK LIST'!$1:$3</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -223,9 +222,6 @@
   </si>
   <si>
     <t>AREA/PACAL</t>
-  </si>
-  <si>
-    <t>Ing. Jenny Alexandra Ruiz Robalino</t>
   </si>
   <si>
     <t>N°</t>
@@ -525,11 +521,14 @@
   <si>
     <t>22/2024</t>
   </si>
+  <si>
+    <t>Bryan Patiño</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
@@ -1104,7 +1103,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1282,24 +1281,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1354,20 +1353,23 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="11" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="12">
-    <cellStyle name="Bueno 2" xfId="5" xr:uid="{537BBBE7-B876-4A4D-B120-536D0A49E69E}"/>
+    <cellStyle name="Bueno 2" xfId="5"/>
     <cellStyle name="Encabezado 1" xfId="11" builtinId="16"/>
-    <cellStyle name="Incorrecto 2" xfId="8" xr:uid="{1D05D9CA-6DFA-4C6B-BE44-BA03EC137C3E}"/>
-    <cellStyle name="Neutral 2" xfId="6" xr:uid="{6E210EB5-B923-490A-9CB5-210050F5E4F4}"/>
+    <cellStyle name="Incorrecto 2" xfId="8"/>
+    <cellStyle name="Neutral 2" xfId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{4FB40E68-C915-4C9E-A7E7-E2208B122AAA}"/>
-    <cellStyle name="Normal 2 2" xfId="4" xr:uid="{121694B6-DC8C-41A8-9841-DBC43409A9E6}"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{B87D193D-2060-49A5-B9F0-3410D43909DC}"/>
-    <cellStyle name="Normal 4" xfId="10" xr:uid="{D52D5CA9-9CC8-4DAE-A1FB-8354590B449C}"/>
-    <cellStyle name="Normal 5" xfId="3" xr:uid="{F9A3F5A3-D783-4CB6-8C09-2CEEF5B0599C}"/>
-    <cellStyle name="Notas 2" xfId="9" xr:uid="{3D5821DD-315F-440E-8D01-A9CF9B62E144}"/>
-    <cellStyle name="Porcentaje 2" xfId="7" xr:uid="{28511EFB-E51E-4F82-B35A-CB057CA424A6}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2 2" xfId="4"/>
+    <cellStyle name="Normal 3" xfId="1"/>
+    <cellStyle name="Normal 4" xfId="10"/>
+    <cellStyle name="Normal 5" xfId="3"/>
+    <cellStyle name="Notas 2" xfId="9"/>
+    <cellStyle name="Porcentaje 2" xfId="7"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1678,7 +1680,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA3B471-17CF-4451-8693-C4E016F92883}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1699,52 +1701,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17">
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
     </row>
     <row r="2" spans="2:17" ht="25.8" customHeight="1">
-      <c r="B2" s="70" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="70"/>
+      <c r="B2" s="69" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="69"/>
+      <c r="P2" s="69"/>
+      <c r="Q2" s="69"/>
     </row>
     <row r="3" spans="2:17">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="72"/>
+      <c r="C3" s="71"/>
       <c r="D3" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E3" s="73" t="s">
         <v>12</v>
@@ -1752,12 +1754,12 @@
       <c r="F3" s="74"/>
     </row>
     <row r="4" spans="2:17">
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="72"/>
+      <c r="C4" s="71"/>
       <c r="D4" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E4" s="73" t="s">
         <v>12</v>
@@ -1765,12 +1767,12 @@
       <c r="F4" s="74"/>
     </row>
     <row r="5" spans="2:17">
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="72"/>
+      <c r="C5" s="71"/>
       <c r="D5" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" s="73" t="s">
         <v>12</v>
@@ -1778,18 +1780,18 @@
       <c r="F5" s="74"/>
     </row>
     <row r="6" spans="2:17">
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="72"/>
+      <c r="C6" s="71"/>
       <c r="D6" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E6" s="73" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="74"/>
-      <c r="G6" s="72">
+      <c r="G6" s="71">
         <v>2023</v>
       </c>
       <c r="H6" s="75"/>
@@ -1801,44 +1803,44 @@
       <c r="N6" s="75"/>
       <c r="O6" s="75"/>
       <c r="P6" s="75"/>
-      <c r="Q6" s="68" t="s">
+      <c r="Q6" s="67" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="2:17">
       <c r="E7" s="64"/>
       <c r="F7" s="65"/>
-      <c r="G7" s="67" t="s">
+      <c r="G7" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="67" t="s">
+      <c r="H7" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="67" t="s">
+      <c r="I7" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="67" t="s">
+      <c r="J7" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="67" t="s">
+      <c r="K7" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="67" t="s">
+      <c r="L7" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="67" t="s">
+      <c r="M7" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="N7" s="67" t="s">
+      <c r="N7" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="O7" s="67" t="s">
+      <c r="O7" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="P7" s="67" t="s">
+      <c r="P7" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="Q7" s="68"/>
+      <c r="Q7" s="67"/>
     </row>
     <row r="8" spans="2:17">
       <c r="B8" s="6" t="s">
@@ -1856,17 +1858,17 @@
       <c r="F8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="67"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="67"/>
-      <c r="J8" s="67"/>
-      <c r="K8" s="67"/>
-      <c r="L8" s="67"/>
-      <c r="M8" s="67"/>
-      <c r="N8" s="67"/>
-      <c r="O8" s="67"/>
-      <c r="P8" s="67"/>
-      <c r="Q8" s="68"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="72"/>
+      <c r="L8" s="72"/>
+      <c r="M8" s="72"/>
+      <c r="N8" s="72"/>
+      <c r="O8" s="72"/>
+      <c r="P8" s="72"/>
+      <c r="Q8" s="67"/>
     </row>
     <row r="9" spans="2:17" s="2" customFormat="1" ht="99.9" customHeight="1">
       <c r="B9" s="5" t="s">
@@ -1879,10 +1881,10 @@
         <v>6</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="3"/>
@@ -1907,10 +1909,10 @@
         <v>6</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="3"/>
@@ -1935,10 +1937,10 @@
         <v>6</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="3" t="s">
@@ -1965,10 +1967,10 @@
         <v>6</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="3"/>
@@ -1993,10 +1995,10 @@
         <v>6</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="3"/>
@@ -2021,10 +2023,10 @@
         <v>6</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="3" t="s">
@@ -2045,6 +2047,12 @@
     <row r="17" s="2" customFormat="1" ht="99.9" customHeight="1"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
     <mergeCell ref="Q6:Q8"/>
     <mergeCell ref="B1:Q1"/>
     <mergeCell ref="B2:Q2"/>
@@ -2061,12 +2069,6 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="G6:P6"/>
     <mergeCell ref="G7:G8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -2075,11 +2077,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BC422AF-D626-4C6F-A609-BD2ACA92CE0C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A17" zoomScale="90" zoomScaleNormal="70" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="90" zoomScaleNormal="70" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -2203,7 +2205,7 @@
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1">
       <c r="A12" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
@@ -2257,22 +2259,22 @@
         <v>45483</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E15" s="40" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F15" s="66" t="s">
-        <v>81</v>
-      </c>
-      <c r="G15" s="28" t="s">
-        <v>58</v>
+        <v>80</v>
+      </c>
+      <c r="G15" s="91" t="s">
+        <v>109</v>
       </c>
       <c r="H15" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="147.6" customHeight="1">
@@ -2281,22 +2283,22 @@
         <v>45488</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E16" s="40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F16" s="66" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G16" s="28" t="s">
-        <v>58</v>
+        <v>109</v>
       </c>
       <c r="H16" s="27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I16" s="22"/>
     </row>
@@ -2306,47 +2308,47 @@
         <v>45490</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E17" s="40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F17" s="66" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G17" s="28" t="s">
-        <v>58</v>
+        <v>109</v>
       </c>
       <c r="H17" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I17" s="23"/>
     </row>
     <row r="18" spans="1:9" ht="102" customHeight="1">
       <c r="A18" s="88"/>
       <c r="B18" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18" s="66" t="s">
+        <v>83</v>
+      </c>
+      <c r="G18" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="C18" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="E18" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="F18" s="66" t="s">
-        <v>84</v>
-      </c>
-      <c r="G18" s="28" t="s">
-        <v>58</v>
-      </c>
       <c r="H18" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I18" s="22"/>
     </row>
@@ -2356,22 +2358,22 @@
         <v>45497</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E19" s="40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F19" s="66" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G19" s="28" t="s">
-        <v>58</v>
+        <v>109</v>
       </c>
       <c r="H19" s="29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I19" s="23"/>
     </row>
@@ -2432,7 +2434,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85F2A071-9CCC-413D-BB7B-757E3337BD3F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I11"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="110" zoomScaleNormal="80" zoomScaleSheetLayoutView="110" workbookViewId="0">
@@ -2454,7 +2456,7 @@
   <sheetData>
     <row r="1" spans="2:9" ht="20.399999999999999" thickBot="1">
       <c r="B1" s="90" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C1" s="90"/>
       <c r="D1" s="90"/>
@@ -2467,28 +2469,28 @@
     <row r="2" spans="2:9" ht="15" thickTop="1"/>
     <row r="3" spans="2:9" ht="27.6">
       <c r="B3" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="62" t="s">
+      <c r="D3" s="62" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="62" t="s">
+      <c r="E3" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="63" t="s">
+      <c r="F3" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="F3" s="62" t="s">
+      <c r="G3" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="G3" s="63" t="s">
+      <c r="H3" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="H3" s="63" t="s">
+      <c r="I3" s="63" t="s">
         <v>65</v>
-      </c>
-      <c r="I3" s="63" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="200.1" customHeight="1">
@@ -2499,16 +2501,16 @@
         <v>33</v>
       </c>
       <c r="D4" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="F4" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="F4" s="56" t="s">
+      <c r="G4" s="56" t="s">
         <v>69</v>
-      </c>
-      <c r="G4" s="56" t="s">
-        <v>70</v>
       </c>
       <c r="H4" s="57" t="s">
         <v>34</v>
@@ -2525,16 +2527,16 @@
         <v>35</v>
       </c>
       <c r="D5" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="E5" s="45" t="s">
+      <c r="F5" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="F5" s="45" t="s">
-        <v>69</v>
-      </c>
       <c r="G5" s="45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H5" s="46" t="s">
         <v>36</v>
@@ -2549,16 +2551,16 @@
         <v>37</v>
       </c>
       <c r="D6" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="E6" s="45" t="s">
+      <c r="F6" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="F6" s="45" t="s">
-        <v>69</v>
-      </c>
       <c r="G6" s="45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H6" s="46" t="s">
         <v>38</v>
@@ -2573,16 +2575,16 @@
         <v>39</v>
       </c>
       <c r="D7" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="F7" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="F7" s="45" t="s">
-        <v>69</v>
-      </c>
       <c r="G7" s="45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H7" s="46" t="s">
         <v>40</v>
@@ -2597,16 +2599,16 @@
         <v>41</v>
       </c>
       <c r="D8" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="E8" s="49" t="s">
+      <c r="F8" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="F8" s="49" t="s">
-        <v>69</v>
-      </c>
       <c r="G8" s="49" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H8" s="50" t="s">
         <v>42</v>
@@ -2621,16 +2623,16 @@
         <v>43</v>
       </c>
       <c r="D9" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="53" t="s">
-        <v>68</v>
-      </c>
       <c r="F9" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" s="53" t="s">
         <v>75</v>
-      </c>
-      <c r="G9" s="53" t="s">
-        <v>76</v>
       </c>
       <c r="H9" s="54" t="s">
         <v>44</v>
@@ -2645,16 +2647,16 @@
         <v>45</v>
       </c>
       <c r="D10" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="56" t="s">
-        <v>68</v>
-      </c>
       <c r="F10" s="56" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G10" s="56" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H10" s="57" t="s">
         <v>46</v>
@@ -2669,16 +2671,16 @@
         <v>47</v>
       </c>
       <c r="D11" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="E11" s="45" t="s">
-        <v>68</v>
-      </c>
       <c r="F11" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="45" t="s">
         <v>78</v>
-      </c>
-      <c r="G11" s="45" t="s">
-        <v>79</v>
       </c>
       <c r="H11" s="46" t="s">
         <v>48</v>

</xml_diff>